<commit_message>
updates of excel with targets and clinical trials
</commit_message>
<xml_diff>
--- a/cartcontent/Clinical trials and cancer types per CART target.xlsx
+++ b/cartcontent/Clinical trials and cancer types per CART target.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gimo/Dropbox/PhD/Projects/CarT/Analyses/biosurf2024/cartcontent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9765F882-CF8C-1946-912A-60AC79544392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3037A4C9-118D-2D46-A186-ED376991D4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4E4F2C52-7944-A244-8554-531799460318}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="202">
   <si>
     <t>Target</t>
   </si>
@@ -564,6 +564,84 @@
   </si>
   <si>
     <t>NCT04661384</t>
+  </si>
+  <si>
+    <t>NCT04483778</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/study/NCT04483778?term=cd19&amp;intr=CAR-T&amp;cond=Cancer&amp;page=29&amp;rank=285</t>
+  </si>
+  <si>
+    <t>Retinoblastoma</t>
+  </si>
+  <si>
+    <t>Hepatoblastoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NCT04488354</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/study/NCT04488354?term=cd19&amp;intr=CAR-T&amp;cond=Cancer&amp;page=31&amp;rank=302</t>
+  </si>
+  <si>
+    <t>Waldenstrom Macroglobulinemia</t>
+  </si>
+  <si>
+    <t>NCT02208362</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/study/NCT02208362?term=cd19&amp;intr=CAR-T&amp;cond=Cancer&amp;page=42&amp;rank=417</t>
+  </si>
+  <si>
+    <t>Melanoma</t>
+  </si>
+  <si>
+    <t>Neuroendocrine Tumors</t>
+  </si>
+  <si>
+    <t>Paraganglioma</t>
+  </si>
+  <si>
+    <t>Adrenocortical Carcinoma</t>
+  </si>
+  <si>
+    <t>Thyroid Cancer</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/study/NCT04119024?term=cd19&amp;intr=CAR-T&amp;cond=Cancer&amp;page=43&amp;rank=427</t>
+  </si>
+  <si>
+    <t>NCT04119024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not sure if relevant. I don't fully understand description. Read again. </t>
+  </si>
+  <si>
+    <t>Sarcoma</t>
+  </si>
+  <si>
+    <t>Neuroblastoma</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/study/NCT03618381?term=cd19&amp;intr=CAR-T&amp;cond=Cancer&amp;page=44&amp;rank=431</t>
+  </si>
+  <si>
+    <t>NCT03618381</t>
+  </si>
+  <si>
+    <t>NCT02465983</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/study/NCT02465983?term=cd19&amp;intr=CAR-T&amp;cond=Cancer&amp;page=45&amp;rank=448</t>
+  </si>
+  <si>
+    <t>NCT02624258</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/study/NCT02624258?term=cd19&amp;intr=CAR-T&amp;cond=Cancer&amp;page=46&amp;rank=458</t>
+  </si>
+  <si>
+    <t>Hodgkin Lymphoma</t>
   </si>
 </sst>
 </file>
@@ -693,19 +771,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -714,9 +786,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -724,25 +793,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -754,40 +805,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -795,13 +815,91 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1138,28 +1236,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29B0FA6-9684-F941-9B84-FA05BE362181}">
-  <dimension ref="A1:K117"/>
+  <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="15.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="24" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="24"/>
+    <col min="5" max="5" width="15.6640625" style="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
       <c r="I1" s="1" t="s">
         <v>100</v>
       </c>
@@ -1167,19 +1265,19 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="1"/>
@@ -1187,19 +1285,19 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="37" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="1"/>
@@ -1207,45 +1305,45 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="37"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="11" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="37"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="1"/>
@@ -1253,1217 +1351,1383 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="11" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="9"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="11" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="13"/>
+      <c r="E9" s="37"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="37"/>
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="13"/>
+      <c r="E13" s="37"/>
     </row>
     <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="37" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="11" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="18"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="37"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="17"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="11" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="17"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="11" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="11" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="11" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="18"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="11" t="s">
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="18"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10" t="s">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="37" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="23"/>
+      <c r="E27" s="38"/>
     </row>
     <row r="28" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21" t="s">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="38"/>
     </row>
     <row r="29" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
-      <c r="B29" s="24" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="26"/>
+      <c r="E29" s="39"/>
     </row>
     <row r="30" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
-      <c r="B30" s="24" t="s">
+      <c r="A30" s="10"/>
+      <c r="B30" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="26"/>
+      <c r="E30" s="39"/>
     </row>
     <row r="31" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20" t="s">
+      <c r="A31" s="10"/>
+      <c r="B31" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="38" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="19"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21" t="s">
+      <c r="A32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="23"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="38"/>
     </row>
     <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="23"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="38"/>
     </row>
     <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="19"/>
-      <c r="B34" s="24" t="s">
+      <c r="A34" s="10"/>
+      <c r="B34" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="26"/>
+      <c r="E34" s="39"/>
     </row>
     <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20" t="s">
+      <c r="A35" s="10"/>
+      <c r="B35" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="23"/>
+      <c r="E35" s="38"/>
     </row>
     <row r="36" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="19"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21" t="s">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="23"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="38"/>
     </row>
     <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="19"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21" t="s">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="23"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="38"/>
     </row>
     <row r="38" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="19"/>
-      <c r="B38" s="20" t="s">
+      <c r="A38" s="10"/>
+      <c r="B38" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="E38" s="23"/>
+      <c r="E38" s="38"/>
     </row>
     <row r="39" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21" t="s">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="23"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="38"/>
     </row>
     <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21" t="s">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="23"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="38"/>
     </row>
     <row r="41" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="19"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="21" t="s">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="23"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="13"/>
+      <c r="E42" s="37"/>
     </row>
     <row r="43" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="11" t="s">
+      <c r="A43" s="6"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="15"/>
-      <c r="E43" s="13"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="37"/>
     </row>
     <row r="44" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="9"/>
-      <c r="B44" s="14" t="s">
+      <c r="A44" s="6"/>
+      <c r="B44" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="13"/>
+      <c r="E44" s="37"/>
     </row>
     <row r="45" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="9"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="11" t="s">
+      <c r="A45" s="6"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="13"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="37"/>
     </row>
     <row r="46" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="9"/>
-      <c r="B46" s="10" t="s">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="13"/>
+      <c r="E46" s="37"/>
     </row>
     <row r="47" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="9"/>
-      <c r="B47" s="10" t="s">
+      <c r="A47" s="6"/>
+      <c r="B47" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="E47" s="13"/>
+      <c r="E47" s="37"/>
     </row>
     <row r="48" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="9"/>
-      <c r="B48" s="10" t="s">
+      <c r="A48" s="6"/>
+      <c r="B48" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="E48" s="13"/>
+      <c r="E48" s="37"/>
     </row>
     <row r="49" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="9"/>
-      <c r="B49" s="10" t="s">
+      <c r="A49" s="6"/>
+      <c r="B49" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E49" s="37" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="9"/>
-      <c r="B50" s="10" t="s">
+      <c r="A50" s="6"/>
+      <c r="B50" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="13"/>
+      <c r="E50" s="37"/>
     </row>
     <row r="51" spans="1:5" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="9"/>
-      <c r="B51" s="10" t="s">
+      <c r="A51" s="6"/>
+      <c r="B51" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="37" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="9"/>
-      <c r="B52" s="10" t="s">
+      <c r="A52" s="6"/>
+      <c r="B52" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D52" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="13"/>
+      <c r="E52" s="37"/>
     </row>
     <row r="53" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="9"/>
-      <c r="B53" s="10" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="E53" s="13"/>
+      <c r="E53" s="37"/>
     </row>
     <row r="54" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="9"/>
-      <c r="B54" s="14" t="s">
+      <c r="A54" s="6"/>
+      <c r="B54" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="E54" s="13"/>
+      <c r="E54" s="37"/>
     </row>
     <row r="55" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="9"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="11" t="s">
+      <c r="A55" s="6"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D55" s="16"/>
-      <c r="E55" s="13"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="37"/>
     </row>
     <row r="56" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="9"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="11" t="s">
+      <c r="A56" s="6"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="13"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="37"/>
     </row>
     <row r="57" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="9"/>
-      <c r="B57" s="10" t="s">
+      <c r="A57" s="6"/>
+      <c r="B57" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="E57" s="13"/>
+      <c r="E57" s="37"/>
     </row>
     <row r="58" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="9"/>
-      <c r="B58" s="10" t="s">
+      <c r="A58" s="6"/>
+      <c r="B58" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="E58" s="13"/>
+      <c r="E58" s="37"/>
     </row>
     <row r="59" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="9"/>
-      <c r="B59" s="10" t="s">
+      <c r="A59" s="6"/>
+      <c r="B59" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="E59" s="13"/>
+      <c r="E59" s="37"/>
     </row>
     <row r="60" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9" t="s">
+      <c r="A60" s="6"/>
+      <c r="B60" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="D60" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="E60" s="13"/>
+      <c r="E60" s="37"/>
     </row>
     <row r="61" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="11" t="s">
+      <c r="A61" s="6"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D61" s="16"/>
-      <c r="E61" s="13"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="37"/>
     </row>
     <row r="62" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="11" t="s">
+      <c r="A62" s="6"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D62" s="16"/>
-      <c r="E62" s="13"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="37"/>
     </row>
     <row r="63" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="9"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="11" t="s">
+      <c r="A63" s="6"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D63" s="16"/>
-      <c r="E63" s="13"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="37"/>
     </row>
     <row r="64" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="11" t="s">
+      <c r="A64" s="6"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D64" s="16"/>
-      <c r="E64" s="13"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="37"/>
     </row>
     <row r="65" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="9"/>
-      <c r="B65" s="14" t="s">
+      <c r="A65" s="6"/>
+      <c r="B65" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="D65" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="E65" s="13"/>
+      <c r="E65" s="37"/>
     </row>
     <row r="66" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="9"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="11" t="s">
+      <c r="A66" s="6"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D66" s="16"/>
-      <c r="E66" s="13"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="37"/>
     </row>
     <row r="67" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="9"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="11" t="s">
+      <c r="A67" s="6"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D67" s="16"/>
-      <c r="E67" s="13"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="37"/>
     </row>
     <row r="68" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="9"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="11" t="s">
+      <c r="A68" s="6"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="13"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="37"/>
     </row>
     <row r="69" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="9"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="11" t="s">
+      <c r="A69" s="6"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D69" s="16"/>
-      <c r="E69" s="13"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="37"/>
     </row>
     <row r="70" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="9"/>
-      <c r="B70" s="14" t="s">
+      <c r="A70" s="6"/>
+      <c r="B70" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D70" s="15" t="s">
+      <c r="D70" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="E70" s="13"/>
+      <c r="E70" s="37"/>
     </row>
     <row r="71" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="9"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="11" t="s">
+      <c r="A71" s="6"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D71" s="16"/>
-      <c r="E71" s="13"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="37"/>
     </row>
     <row r="72" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="9"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="11" t="s">
+      <c r="A72" s="6"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D72" s="16"/>
-      <c r="E72" s="13"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="37"/>
     </row>
     <row r="73" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="9"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="11" t="s">
+      <c r="A73" s="6"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D73" s="16"/>
-      <c r="E73" s="13"/>
+      <c r="D73" s="27"/>
+      <c r="E73" s="37"/>
     </row>
     <row r="74" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="9"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="11" t="s">
+      <c r="A74" s="6"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D74" s="16"/>
-      <c r="E74" s="13"/>
+      <c r="D74" s="27"/>
+      <c r="E74" s="37"/>
     </row>
     <row r="75" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="9"/>
-      <c r="B75" s="14" t="s">
+      <c r="A75" s="6"/>
+      <c r="B75" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D75" s="27" t="s">
+      <c r="D75" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E75" s="13"/>
+      <c r="E75" s="37"/>
     </row>
     <row r="76" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="9"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="11" t="s">
+      <c r="A76" s="6"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D76" s="27"/>
-      <c r="E76" s="13"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="37"/>
     </row>
     <row r="77" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="9"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="11" t="s">
+      <c r="A77" s="6"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D77" s="27"/>
-      <c r="E77" s="13"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="37"/>
     </row>
     <row r="78" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="9"/>
-      <c r="B78" s="14"/>
-      <c r="C78" s="11" t="s">
+      <c r="A78" s="6"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="D78" s="27"/>
-      <c r="E78" s="13"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="37"/>
     </row>
     <row r="79" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="9"/>
-      <c r="B79" s="14"/>
-      <c r="C79" s="11" t="s">
+      <c r="A79" s="6"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D79" s="27"/>
-      <c r="E79" s="13"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="37"/>
     </row>
     <row r="80" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="9"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="11" t="s">
+      <c r="A80" s="6"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D80" s="27"/>
-      <c r="E80" s="13"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="37"/>
     </row>
     <row r="81" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="9"/>
-      <c r="B81" s="14"/>
-      <c r="C81" s="11" t="s">
+      <c r="A81" s="6"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D81" s="27"/>
-      <c r="E81" s="13"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="37"/>
     </row>
     <row r="82" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="9"/>
-      <c r="B82" s="14" t="s">
+      <c r="A82" s="6"/>
+      <c r="B82" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C82" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="D82" s="11"/>
-      <c r="E82" s="13"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="37"/>
     </row>
     <row r="83" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="9"/>
-      <c r="B83" s="14"/>
-      <c r="C83" s="11" t="s">
+      <c r="A83" s="6"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D83" s="11"/>
-      <c r="E83" s="13"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="37"/>
     </row>
     <row r="84" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="29" t="s">
+      <c r="A84" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B84" s="34" t="s">
+      <c r="B84" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="C84" s="21" t="s">
+      <c r="C84" s="23" t="s">
         <v>137</v>
       </c>
       <c r="D84" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="E84" s="26"/>
+      <c r="E84" s="39"/>
     </row>
     <row r="85" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="28"/>
-      <c r="B85" s="35"/>
-      <c r="C85" s="21" t="s">
+      <c r="A85" s="19"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D85" s="30"/>
-      <c r="E85" s="26"/>
+      <c r="D85" s="32"/>
+      <c r="E85" s="39"/>
     </row>
     <row r="86" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="28"/>
-      <c r="B86" s="34" t="s">
+      <c r="A86" s="19"/>
+      <c r="B86" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="C86" s="21" t="s">
+      <c r="C86" s="23" t="s">
         <v>137</v>
       </c>
       <c r="D86" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="E86" s="26"/>
+      <c r="E86" s="39"/>
     </row>
     <row r="87" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="28"/>
-      <c r="B87" s="35"/>
-      <c r="C87" s="21" t="s">
+      <c r="A87" s="19"/>
+      <c r="B87" s="15"/>
+      <c r="C87" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D87" s="30"/>
-      <c r="E87" s="26"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="39"/>
     </row>
     <row r="88" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="28"/>
-      <c r="B88" s="34" t="s">
+      <c r="A88" s="19"/>
+      <c r="B88" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C88" s="21" t="s">
+      <c r="C88" s="23" t="s">
         <v>137</v>
       </c>
       <c r="D88" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="E88" s="26"/>
+      <c r="E88" s="39"/>
     </row>
     <row r="89" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="28"/>
-      <c r="B89" s="38"/>
-      <c r="C89" s="21" t="s">
+      <c r="A89" s="19"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D89" s="36"/>
-      <c r="E89" s="26"/>
+      <c r="D89" s="33"/>
+      <c r="E89" s="39"/>
     </row>
     <row r="90" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="28"/>
-      <c r="B90" s="35"/>
-      <c r="C90" s="21" t="s">
+      <c r="A90" s="19"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D90" s="30"/>
-      <c r="E90" s="26"/>
+      <c r="D90" s="32"/>
+      <c r="E90" s="39"/>
     </row>
     <row r="91" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="28"/>
-      <c r="B91" s="24" t="s">
+      <c r="A91" s="19"/>
+      <c r="B91" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="C91" s="21" t="s">
+      <c r="C91" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D91" s="25" t="s">
+      <c r="D91" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="E91" s="26"/>
+      <c r="E91" s="39"/>
     </row>
     <row r="92" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="28"/>
-      <c r="B92" s="24" t="s">
+      <c r="A92" s="19"/>
+      <c r="B92" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="C92" s="21" t="s">
+      <c r="C92" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="D92" s="25" t="s">
+      <c r="D92" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="E92" s="26"/>
+      <c r="E92" s="39"/>
     </row>
     <row r="93" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="28"/>
-      <c r="B93" s="34" t="s">
+      <c r="A93" s="19"/>
+      <c r="B93" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C93" s="21" t="s">
+      <c r="C93" s="23" t="s">
         <v>55</v>
       </c>
       <c r="D93" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="E93" s="26"/>
+      <c r="E93" s="39"/>
     </row>
     <row r="94" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="28"/>
-      <c r="B94" s="35"/>
-      <c r="C94" s="21" t="s">
+      <c r="A94" s="19"/>
+      <c r="B94" s="15"/>
+      <c r="C94" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D94" s="30"/>
-      <c r="E94" s="26"/>
+      <c r="D94" s="32"/>
+      <c r="E94" s="39"/>
     </row>
     <row r="95" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="28"/>
-      <c r="B95" s="24" t="s">
+      <c r="A95" s="19"/>
+      <c r="B95" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C95" s="21" t="s">
+      <c r="C95" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="D95" s="25" t="s">
+      <c r="D95" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="E95" s="26"/>
+      <c r="E95" s="39"/>
     </row>
     <row r="96" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="28"/>
-      <c r="B96" s="24" t="s">
+      <c r="A96" s="19"/>
+      <c r="B96" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="C96" s="21" t="s">
+      <c r="C96" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="D96" s="25" t="s">
+      <c r="D96" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="E96" s="26"/>
+      <c r="E96" s="39"/>
     </row>
     <row r="97" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="28"/>
-      <c r="B97" s="24" t="s">
+      <c r="A97" s="19"/>
+      <c r="B97" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="C97" s="21" t="s">
+      <c r="C97" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="D97" s="25" t="s">
+      <c r="D97" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="E97" s="26"/>
+      <c r="E97" s="39"/>
     </row>
     <row r="98" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="28"/>
-      <c r="B98" s="24" t="s">
+      <c r="A98" s="19"/>
+      <c r="B98" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="C98" s="21" t="s">
+      <c r="C98" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="D98" s="25" t="s">
+      <c r="D98" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="E98" s="26"/>
+      <c r="E98" s="39"/>
     </row>
     <row r="99" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="28"/>
-      <c r="B99" s="34" t="s">
+      <c r="A99" s="19"/>
+      <c r="B99" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C99" s="21" t="s">
+      <c r="C99" s="23" t="s">
         <v>38</v>
       </c>
       <c r="D99" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="E99" s="26"/>
+      <c r="E99" s="39"/>
     </row>
     <row r="100" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="28"/>
-      <c r="B100" s="35"/>
-      <c r="C100" s="21" t="s">
+      <c r="A100" s="19"/>
+      <c r="B100" s="15"/>
+      <c r="C100" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D100" s="30"/>
-      <c r="E100" s="26"/>
+      <c r="D100" s="32"/>
+      <c r="E100" s="39"/>
     </row>
     <row r="101" spans="1:5" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="28"/>
-      <c r="B101" s="24" t="s">
+      <c r="A101" s="19"/>
+      <c r="B101" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C101" s="21" t="s">
+      <c r="C101" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D101" s="25" t="s">
+      <c r="D101" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="E101" s="26" t="s">
+      <c r="E101" s="39" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="28"/>
-      <c r="B102" s="32" t="s">
+      <c r="A102" s="19"/>
+      <c r="B102" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="C102" s="21" t="s">
+      <c r="C102" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D102" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="E102" s="26"/>
+      <c r="E102" s="39"/>
     </row>
     <row r="103" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="28"/>
-      <c r="B103" s="37"/>
-      <c r="C103" s="21" t="s">
+      <c r="A103" s="19"/>
+      <c r="B103" s="16"/>
+      <c r="C103" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="D103" s="36"/>
-      <c r="E103" s="26"/>
+      <c r="D103" s="33"/>
+      <c r="E103" s="39"/>
     </row>
     <row r="104" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="28"/>
-      <c r="B104" s="33"/>
-      <c r="C104" s="21" t="s">
+      <c r="A104" s="19"/>
+      <c r="B104" s="15"/>
+      <c r="C104" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D104" s="30"/>
-      <c r="E104" s="26"/>
+      <c r="D104" s="32"/>
+      <c r="E104" s="39"/>
     </row>
     <row r="105" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="28"/>
-      <c r="B105" s="24"/>
-      <c r="C105" s="21"/>
-      <c r="D105" s="21"/>
-      <c r="E105" s="26"/>
+      <c r="A105" s="19"/>
+      <c r="B105" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C105" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="D105" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E105" s="39"/>
     </row>
     <row r="106" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="28"/>
-      <c r="B106" s="24"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="21"/>
-      <c r="E106" s="26"/>
+      <c r="A106" s="19"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D106" s="34"/>
+      <c r="E106" s="39"/>
     </row>
     <row r="107" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="28"/>
-      <c r="B107" s="24"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="21"/>
-      <c r="E107" s="26"/>
+      <c r="A107" s="19"/>
+      <c r="B107" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C107" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="D107" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="E107" s="39"/>
     </row>
     <row r="108" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="28"/>
-      <c r="B108" s="24"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="21"/>
-      <c r="E108" s="26"/>
+      <c r="A108" s="19"/>
+      <c r="B108" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C108" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D108" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E108" s="39"/>
     </row>
     <row r="109" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="28"/>
-      <c r="B109" s="24"/>
-      <c r="C109" s="21"/>
-      <c r="D109" s="21"/>
-      <c r="E109" s="26"/>
+      <c r="A109" s="19"/>
+      <c r="B109" s="15"/>
+      <c r="C109" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D109" s="34"/>
+      <c r="E109" s="39"/>
     </row>
     <row r="110" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="28"/>
-      <c r="B110" s="24"/>
-      <c r="C110" s="21"/>
-      <c r="D110" s="21"/>
-      <c r="E110" s="26"/>
+      <c r="A110" s="19"/>
+      <c r="B110" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C110" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D110" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="E110" s="40" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="111" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="28"/>
-      <c r="B111" s="24"/>
-      <c r="C111" s="21"/>
-      <c r="D111" s="21"/>
-      <c r="E111" s="26"/>
+      <c r="A111" s="19"/>
+      <c r="B111" s="16"/>
+      <c r="C111" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D111" s="35"/>
+      <c r="E111" s="41"/>
     </row>
     <row r="112" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="28"/>
-      <c r="B112" s="24"/>
-      <c r="C112" s="21"/>
-      <c r="D112" s="21"/>
-      <c r="E112" s="26"/>
+      <c r="A112" s="19"/>
+      <c r="B112" s="16"/>
+      <c r="C112" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D112" s="35"/>
+      <c r="E112" s="41"/>
     </row>
     <row r="113" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="28"/>
-      <c r="B113" s="24"/>
-      <c r="C113" s="21"/>
-      <c r="D113" s="21"/>
-      <c r="E113" s="26"/>
+      <c r="A113" s="19"/>
+      <c r="B113" s="16"/>
+      <c r="C113" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="D113" s="35"/>
+      <c r="E113" s="41"/>
     </row>
     <row r="114" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="28"/>
-      <c r="B114" s="24"/>
-      <c r="C114" s="21"/>
-      <c r="D114" s="21"/>
-      <c r="E114" s="26"/>
+      <c r="A114" s="19"/>
+      <c r="B114" s="16"/>
+      <c r="C114" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D114" s="35"/>
+      <c r="E114" s="41"/>
     </row>
     <row r="115" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="28"/>
-      <c r="B115" s="24"/>
-      <c r="C115" s="21"/>
-      <c r="D115" s="21"/>
-      <c r="E115" s="26"/>
+      <c r="A115" s="19"/>
+      <c r="B115" s="16"/>
+      <c r="C115" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D115" s="35"/>
+      <c r="E115" s="41"/>
     </row>
     <row r="116" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="28"/>
-      <c r="B116" s="24"/>
-      <c r="C116" s="21"/>
-      <c r="D116" s="21"/>
-      <c r="E116" s="26"/>
+      <c r="A116" s="19"/>
+      <c r="B116" s="15"/>
+      <c r="C116" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D116" s="34"/>
+      <c r="E116" s="42"/>
     </row>
     <row r="117" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="28"/>
-      <c r="B117" s="24"/>
-      <c r="C117" s="21"/>
-      <c r="D117" s="21"/>
-      <c r="E117" s="26"/>
+      <c r="A117" s="19"/>
+      <c r="B117" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C117" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="D117" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="E117" s="43"/>
+    </row>
+    <row r="118" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="19"/>
+      <c r="B118" s="16"/>
+      <c r="C118" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D118" s="35"/>
+      <c r="E118" s="43"/>
+    </row>
+    <row r="119" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="19"/>
+      <c r="B119" s="16"/>
+      <c r="C119" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="D119" s="35"/>
+      <c r="E119" s="43"/>
+    </row>
+    <row r="120" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="19"/>
+      <c r="B120" s="15"/>
+      <c r="C120" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="D120" s="34"/>
+      <c r="E120" s="43"/>
+    </row>
+    <row r="121" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="19"/>
+      <c r="B121" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="C121" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D121" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="E121" s="43"/>
+    </row>
+    <row r="122" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="20"/>
+      <c r="B122" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C122" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="D122" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="E122" s="43"/>
+    </row>
+    <row r="123" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="13"/>
+      <c r="B123" s="17"/>
+      <c r="C123" s="23"/>
+      <c r="D123" s="36"/>
+      <c r="E123" s="43"/>
+    </row>
+    <row r="124" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="13"/>
+      <c r="B124" s="12"/>
+      <c r="C124" s="23"/>
+      <c r="D124" s="23"/>
+      <c r="E124" s="39"/>
+    </row>
+    <row r="125" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="13"/>
+      <c r="B125" s="12"/>
+      <c r="C125" s="23"/>
+      <c r="D125" s="23"/>
+      <c r="E125" s="39"/>
+    </row>
+    <row r="126" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="13"/>
+      <c r="B126" s="12"/>
+      <c r="C126" s="23"/>
+      <c r="D126" s="23"/>
+      <c r="E126" s="39"/>
+    </row>
+    <row r="127" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="13"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="23"/>
+      <c r="D127" s="23"/>
+      <c r="E127" s="39"/>
+    </row>
+    <row r="128" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="13"/>
+      <c r="B128" s="12"/>
+      <c r="C128" s="23"/>
+      <c r="D128" s="23"/>
+      <c r="E128" s="39"/>
+    </row>
+    <row r="129" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="13"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="23"/>
+      <c r="D129" s="23"/>
+      <c r="E129" s="39"/>
+    </row>
+    <row r="130" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="13"/>
+      <c r="B130" s="12"/>
+      <c r="C130" s="23"/>
+      <c r="D130" s="23"/>
+      <c r="E130" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
+  <mergeCells count="68">
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="D110:D116"/>
+    <mergeCell ref="E110:E116"/>
+    <mergeCell ref="B110:B116"/>
+    <mergeCell ref="D117:D120"/>
+    <mergeCell ref="B117:B120"/>
     <mergeCell ref="D99:D100"/>
     <mergeCell ref="B99:B100"/>
     <mergeCell ref="D102:D104"/>
     <mergeCell ref="B102:B104"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="B105:B106"/>
     <mergeCell ref="B86:B87"/>
     <mergeCell ref="D86:D87"/>
     <mergeCell ref="D88:D90"/>
@@ -2476,6 +2740,7 @@
     <mergeCell ref="A42:A83"/>
     <mergeCell ref="D84:D85"/>
     <mergeCell ref="B84:B85"/>
+    <mergeCell ref="A84:A122"/>
     <mergeCell ref="D60:D64"/>
     <mergeCell ref="B60:B64"/>
     <mergeCell ref="B65:B69"/>
@@ -2574,6 +2839,13 @@
     <hyperlink ref="D99" r:id="rId52" xr:uid="{A0EF840E-C36E-7C49-9B59-36219C5D1F16}"/>
     <hyperlink ref="D101" r:id="rId53" xr:uid="{3FEAB4A7-9DB8-9C45-900B-BBA81BEBF9D9}"/>
     <hyperlink ref="D102" r:id="rId54" xr:uid="{CB3037DA-68B6-8945-A03D-41AC3D56A16C}"/>
+    <hyperlink ref="D105" r:id="rId55" xr:uid="{8875D68A-115A-A64B-AB10-626F33F8058C}"/>
+    <hyperlink ref="D107" r:id="rId56" xr:uid="{D35DB35C-F783-ED4C-A336-F3D6D7C0CA2D}"/>
+    <hyperlink ref="D108" r:id="rId57" xr:uid="{718846F5-500B-A84E-AD28-4EB28E33864D}"/>
+    <hyperlink ref="D110" r:id="rId58" xr:uid="{1E6A2E25-8E57-174D-ADC2-E83AFB4B7F99}"/>
+    <hyperlink ref="D117" r:id="rId59" xr:uid="{33AD0126-A894-8948-AA32-28CDB07DA710}"/>
+    <hyperlink ref="D121" r:id="rId60" xr:uid="{7A35D3A2-4B9E-BF4B-81F3-0528AEE90594}"/>
+    <hyperlink ref="D122" r:id="rId61" xr:uid="{1966B3C2-5876-464B-9176-A7E8631C43CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>